<commit_message>
Tambahan Stylized Fact Pertambangan dan Playground Tanner
</commit_message>
<xml_diff>
--- a/doc/Coba Stylized Fact.xlsx
+++ b/doc/Coba Stylized Fact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerja Bismillah\DKEM\KajianFPP\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45565AA-278E-41C6-8908-31DA92DBB460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9786339C-5214-4A62-BABB-77B5A7519060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB5E76F9-A705-4992-8E41-F9C5477B9BFA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -62,25 +62,34 @@
     <t>e</t>
   </si>
   <si>
-    <t>base 1</t>
-  </si>
-  <si>
-    <t>base 2</t>
-  </si>
-  <si>
-    <t>y = m(base 1) + c</t>
-  </si>
-  <si>
-    <t>w = n(base 2) + d</t>
-  </si>
-  <si>
     <t>z</t>
   </si>
   <si>
-    <t>z = o(base 1) + e</t>
+    <t>rumus nilai ekuilibrium bergantung pada input</t>
   </si>
   <si>
-    <t>rumus nilai ekuilibrium bergantung pada input</t>
+    <t>v</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base </t>
+  </si>
+  <si>
+    <t>v = p(base) + f</t>
+  </si>
+  <si>
+    <t>w = n(base) + d</t>
+  </si>
+  <si>
+    <t>y = m(base) + c</t>
+  </si>
+  <si>
+    <t>z = o(base) + e</t>
   </si>
 </sst>
 </file>
@@ -165,10 +174,248 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>w</c:v>
+            <c:v>v</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$10:$L$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-17.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-22.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-27.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-32.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-37.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-42.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-47.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-52.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BCB7-4315-8BCE-75902EC9B401}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>w</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -184,59 +431,204 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!#REF!</c:f>
+              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$10:$K$24</c:f>
+              <c:f>Sheet1!$K$10:$K$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>-2.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>-7.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>-12.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>-17.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-22.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-27.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-32.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-37.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-42.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-47.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-52.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-57.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -250,7 +642,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$F$9</c:f>
@@ -276,53 +668,101 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$24</c:f>
+              <c:f>Sheet1!$E$10:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="18">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="20">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="25">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="26">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="27">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="28">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="29">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="30">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -330,54 +770,102 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$10:$F$24</c:f>
+              <c:f>Sheet1!$F$10:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="22">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="23">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="24">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="25">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="27">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="28">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="29">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="30">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -391,9 +879,17 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>z</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -410,53 +906,101 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$24</c:f>
+              <c:f>Sheet1!$E$10:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="18">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="20">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="25">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="26">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="27">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="28">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="29">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="30">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -464,54 +1008,102 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$10:$G$24</c:f>
+              <c:f>Sheet1!$G$10:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>-45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>-43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>-41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>-39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>-37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>-35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>-33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>-27</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24</c:v>
+                  <c:v>-25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>-23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32</c:v>
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,11 +1117,11 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -545,12 +1137,9 @@
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln w="12700" cap="rnd">
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="40000"/>
-                    <a:lumOff val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:prstDash val="dash"/>
                 <a:round/>
@@ -559,7 +1148,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-98B7-4006-A0C9-D29AF989E883}"/>
+                <c16:uniqueId val="{00000001-887A-4A6F-91E6-0F927CA6C5C6}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -585,10 +1174,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -596,63 +1185,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-288A-48B5-A3B7-255990A21BE6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$32:$B$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$32:$C$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-98B7-4006-A0C9-D29AF989E883}"/>
+              <c16:uniqueId val="{00000005-BCB7-4315-8BCE-75902EC9B401}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -671,7 +1204,8 @@
         <c:axId val="1027139984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15"/>
+          <c:max val="25"/>
+          <c:min val="-25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -713,14 +1247,15 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1027140968"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-25"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1027140968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="40"/>
+          <c:max val="20"/>
+          <c:min val="-25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -756,7 +1291,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1027139984"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-25"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -767,37 +1302,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1736,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A975199-FB5E-4713-850D-869388F6B6C9}">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,79 +2251,86 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>9</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E10">
-        <v>1</v>
+        <v>-15</v>
       </c>
       <c r="F10">
-        <f>$C$12*E10+$C$13</f>
-        <v>2</v>
+        <f t="shared" ref="F10:F17" si="0">$C$12*E10+$C$13</f>
+        <v>-40</v>
       </c>
       <c r="G10">
-        <f>$C$18*E10+$C$19</f>
-        <v>4</v>
-      </c>
-      <c r="J10">
+        <f t="shared" ref="G10:G17" si="1">$C$18*E10+$C$19</f>
+        <v>-45</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K17" si="2">$C$15*-E10+$C$16</f>
+        <v>17.5</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L17" si="3">($C$21*-E10)+$C$22</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>-14</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-38</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-43</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="K10">
-        <f>$C$15*J10+$C$16</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F24" si="0">$C$12*E11+$C$13</f>
-        <v>4</v>
-      </c>
-      <c r="G11">
-        <f>$C$18*E11+$C$19</f>
-        <v>6</v>
-      </c>
-      <c r="J11">
-        <v>14</v>
-      </c>
-      <c r="K11">
-        <f t="shared" ref="K11:K24" si="1">$C$15*J11+$C$16</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -1827,143 +2338,149 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>-13</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-36</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G24" si="2">$C$18*E12+$C$19</f>
-        <v>8</v>
-      </c>
-      <c r="J12">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>-41</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>-12</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-34</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-39</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="J13">
-        <v>12</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E14">
-        <v>5</v>
+        <v>-11</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-32</v>
       </c>
       <c r="G14">
+        <f t="shared" si="1"/>
+        <v>-37</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J14">
-        <v>11</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>-10</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>-30</v>
       </c>
       <c r="G15">
+        <f t="shared" si="1"/>
+        <v>-35</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>-28</v>
       </c>
       <c r="G16">
+        <f t="shared" si="1"/>
+        <v>-33</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="J16">
-        <v>9</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E17">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>-26</v>
       </c>
       <c r="G17">
+        <f t="shared" si="1"/>
+        <v>-31</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1971,210 +2488,550 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>-7</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" ref="F18:F32" si="4">$C$12*E18+$C$13</f>
+        <v>-24</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J18">
-        <v>7</v>
+        <f t="shared" ref="G18:G32" si="5">$C$18*E18+$C$19</f>
+        <v>-29</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K18:K32" si="6">$C$15*-E18+$C$16</f>
+        <v>-2.5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L32" si="7">($C$21*-E18)+$C$22</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>-15</v>
       </c>
       <c r="E19">
+        <v>-6</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>-22</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>-27</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>-5</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>-20</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>-25</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>-7.5</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>2.5</v>
+      </c>
+      <c r="E21">
+        <v>-4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>-18</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>-23</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>-10</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>-15</v>
+      </c>
+      <c r="E22">
+        <v>-3</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>-16</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>-21</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>-12.5</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>-14</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>-19</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>-15</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>-1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>-12</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>-17</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>-17.5</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>-12.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>-15</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>-20</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="J19">
-        <v>6</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J20">
-        <v>5</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="J21">
-        <v>4</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E22">
-        <v>13</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="J22">
-        <v>3</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E23">
-        <v>14</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E24">
-        <v>15</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>-8</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>-13</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>-22.5</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>-17.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>0</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" t="e">
-        <f>(-C13+C16)/(C12-C15)</f>
-        <v>#DIV/0!</v>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>-11</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>-25</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>0</v>
       </c>
       <c r="C28">
+        <f>($C$16-$C$13)/($C$12-$C$15)</f>
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>-9</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>-27.5</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>-22.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" t="e">
-        <f>B28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C29" t="e">
-        <f ca="1">C12((-C13+C16)/(C12-C15))+C13</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f>($C$12*$C$28)+$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>-30</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="7"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>-32.5</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="7"/>
+        <v>-27.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="6"/>
+        <v>-35</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="7"/>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32">
+        <f>C28</f>
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <f>C29</f>
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="6"/>
+        <v>-37.5</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="7"/>
+        <v>-32.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33">
         <v>0</v>
       </c>
-      <c r="C32" t="e">
-        <f ca="1">C29</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="e">
-        <f>B28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" t="e">
-        <f ca="1">C29</f>
-        <v>#REF!</v>
+      <c r="C33">
+        <f>C32</f>
+        <v>30</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F40" si="8">$C$12*E33+$C$13</f>
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G40" si="9">$C$18*E33+$C$19</f>
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ref="K33:K40" si="10">$C$15*-E33+$C$16</f>
+        <v>-40</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L40" si="11">($C$21*-E33)+$C$22</f>
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="10"/>
+        <v>-42.5</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="11"/>
+        <v>-37.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="10"/>
+        <v>-45</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="11"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>11</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="10"/>
+        <v>-47.5</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="11"/>
+        <v>-42.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="10"/>
+        <v>-50</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="11"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="10"/>
+        <v>-52.5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="11"/>
+        <v>-47.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>14</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="10"/>
+        <v>-55</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="11"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="10"/>
+        <v>-57.5</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="11"/>
+        <v>-52.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mengganti grafik Pertambangan dan Stylized Facts Tanner
</commit_message>
<xml_diff>
--- a/doc/Coba Stylized Fact.xlsx
+++ b/doc/Coba Stylized Fact.xlsx
@@ -5,16 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerja Bismillah\DKEM\KajianFPP\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerja Bismillah\DKEM\Riset dan Kajian\KajianFPP\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9786339C-5214-4A62-BABB-77B5A7519060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0F6E01-F25B-438F-83F3-B5A10CD61A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB5E76F9-A705-4992-8E41-F9C5477B9BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="a">Sheet1!$E$12:$E$42</definedName>
+    <definedName name="d">Sheet1!$C$16</definedName>
+    <definedName name="e">Sheet1!$C$19</definedName>
+    <definedName name="f">Sheet1!$C$22</definedName>
+    <definedName name="g">Sheet1!$C$25</definedName>
+    <definedName name="gap">Sheet1!$E$12:$E$42</definedName>
+    <definedName name="h">Sheet1!$C$28</definedName>
+    <definedName name="k">Sheet1!$C$13</definedName>
+    <definedName name="m">Sheet1!$C$12</definedName>
+    <definedName name="n">Sheet1!$C$15</definedName>
+    <definedName name="o">Sheet1!$C$18</definedName>
+    <definedName name="p">Sheet1!$C$21</definedName>
+    <definedName name="q">Sheet1!$C$24</definedName>
+    <definedName name="s">Sheet1!$C$27</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,18 +49,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
-  <si>
-    <t>x</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>y</t>
   </si>
   <si>
     <t>m</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>n</t>
@@ -53,22 +63,10 @@
     <t>d</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>o</t>
   </si>
   <si>
     <t>e</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>rumus nilai ekuilibrium bergantung pada input</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>p</t>
@@ -77,19 +75,58 @@
     <t>f</t>
   </si>
   <si>
-    <t xml:space="preserve">base </t>
+    <t>k</t>
   </si>
   <si>
-    <t>v = p(base) + f</t>
+    <t>y1</t>
   </si>
   <si>
-    <t>w = n(base) + d</t>
+    <t>y2</t>
   </si>
   <si>
-    <t>y = m(base) + c</t>
+    <t>alt i</t>
   </si>
   <si>
-    <t>z = o(base) + e</t>
+    <t>alt (ii)</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>alt (i)</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>alt ii</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>nilai ekuilibrium</t>
   </si>
 </sst>
 </file>
@@ -105,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,8 +155,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -127,14 +182,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -142,6 +355,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF008080"/>
+      <color rgb="FFD60093"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -177,12 +396,12 @@
           <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>v</c:v>
+            <c:v>alt (i) 2</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="008080"/>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -194,7 +413,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -296,102 +515,102 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$10:$L$40</c:f>
+              <c:f>Sheet1!$L$12:$L$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>22.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>17.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>12.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>-2.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>-5</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>-7.5</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="17">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>-12.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="19">
                   <c:v>-15</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="20">
                   <c:v>-17.5</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="21">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="22">
                   <c:v>-22.5</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="23">
                   <c:v>-25</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="24">
                   <c:v>-27.5</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="25">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>-32.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>-35</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
                   <c:v>-37.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="29">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="30">
                   <c:v>-42.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-45</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-47.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-50</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-52.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,20 +626,12 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$K$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>w</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>base 2</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="008080"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -431,7 +642,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -533,7 +744,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$10:$K$40</c:f>
+              <c:f>Sheet1!$K$12:$K$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -645,11 +856,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$9</c:f>
+              <c:f>Sheet1!$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>base</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -657,7 +868,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="D60093"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -668,7 +879,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -770,102 +981,102 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$10:$F$40</c:f>
+              <c:f>Sheet1!$F$12:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>-40</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-38</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-36</c:v>
+                  <c:v>-27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-34</c:v>
+                  <c:v>-25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-32</c:v>
+                  <c:v>-23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-30</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-28</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-26</c:v>
+                  <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-24</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-22</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20</c:v>
+                  <c:v>-11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-18</c:v>
+                  <c:v>-9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-16</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-14</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-12</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-10</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>18</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -882,11 +1093,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$9</c:f>
+              <c:f>Sheet1!$G$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>alt (i)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -894,7 +1105,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="D60093"/>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -906,7 +1117,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$40</c:f>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -1008,7 +1219,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$10:$G$40</c:f>
+              <c:f>Sheet1!$G$12:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -1118,6 +1329,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>Series 4</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="9525" cap="rnd">
               <a:solidFill>
@@ -1154,30 +1368,30 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$B$29</c:f>
+              <c:f>Sheet1!$B$36:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-4.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-4.2222222222222223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$28:$C$29</c:f>
+              <c:f>Sheet1!$C$36:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>-25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>-9.4444444444444446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,6 +1400,1172 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-BCB7-4315-8BCE-75902EC9B401}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Series 5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$40:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-9.4444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.4444444444444446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5143-4F9F-BD21-D048AFE020BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Series 6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$44:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$44:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.555555555555555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5143-4F9F-BD21-D048AFE020BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Series 7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$48:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$48:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-10.555555555555555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.555555555555555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5143-4F9F-BD21-D048AFE020BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>alt (ii)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="D60093"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$12:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>alt (ii) 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="008080"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$12:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$12:$M$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-7.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-17.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-22.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-27.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$52:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.1111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1111111111111112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$52:$C$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1111111111111112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$56:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>base title</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>base</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$61:$B$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-4.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$61:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-9.4444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.4444444444444446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>alt (i) title</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>alt</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (i)</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$65:$B$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$65:$C$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-10.555555555555555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.555555555555555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D873-4E8D-93FE-DFB7F1FC2410}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:v>alt (ii) title</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>alt</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (ii)</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-D873-4E8D-93FE-DFB7F1FC2410}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$69:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.1111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1111111111111112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$69:$C$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-D873-4E8D-93FE-DFB7F1FC2410}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1907,15 +3287,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:colOff>444137</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>11248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139337</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>11248</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2240,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A975199-FB5E-4713-850D-869388F6B6C9}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2251,792 +3631,1406 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2">
+        <f>(-k + d)/(m+n)</f>
+        <v>-4.2222222222222223</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="15"/>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <f>m*((-k + d)/(m+n))+k</f>
+        <v>-9.4444444444444446</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="12">
+        <f xml:space="preserve"> (-e+f)/(o+p)</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <f xml:space="preserve"> o*((-e+f)/(o+p)) + e</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8">
+        <f>(-g + h)/(q+s)</f>
+        <v>3.1111111111111112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="21"/>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <f>q*((-g + h)/(q+s))+g</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>-15</v>
+      </c>
+      <c r="F12">
+        <f>m*gap+k</f>
+        <v>-31</v>
+      </c>
+      <c r="G12">
+        <f>o*gap+e</f>
+        <v>-45</v>
+      </c>
+      <c r="H12">
+        <f>q*gap+g</f>
+        <v>-34</v>
+      </c>
+      <c r="K12">
+        <f>n*-gap+d</f>
+        <v>17.5</v>
+      </c>
+      <c r="L12">
+        <f>(p*-gap)+f</f>
+        <v>32.5</v>
+      </c>
+      <c r="M12">
+        <f>(s*-gap)+h</f>
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>-14</v>
+      </c>
+      <c r="F13">
+        <f>m*gap+k</f>
+        <v>-29</v>
+      </c>
+      <c r="G13">
+        <f>o*gap+e</f>
+        <v>-43</v>
+      </c>
+      <c r="H13">
+        <f>q*gap+g</f>
+        <v>-32</v>
+      </c>
+      <c r="K13">
+        <f>n*-gap+d</f>
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <f>(p*-gap)+f</f>
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <f>(s*-gap)+h</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="E14">
+        <v>-13</v>
+      </c>
+      <c r="F14">
+        <f>m*gap+k</f>
+        <v>-27</v>
+      </c>
+      <c r="G14">
+        <f>o*gap+e</f>
+        <v>-41</v>
+      </c>
+      <c r="H14">
+        <f>q*gap+g</f>
+        <v>-30</v>
+      </c>
+      <c r="K14">
+        <f>n*-gap+d</f>
+        <v>12.5</v>
+      </c>
+      <c r="L14">
+        <f>(p*-gap)+f</f>
+        <v>27.5</v>
+      </c>
+      <c r="M14">
+        <f>(s*-gap)+h</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E15">
+        <v>-12</v>
+      </c>
+      <c r="F15">
+        <f>m*gap+k</f>
+        <v>-25</v>
+      </c>
+      <c r="G15">
+        <f>o*gap+e</f>
+        <v>-39</v>
+      </c>
+      <c r="H15">
+        <f>q*gap+g</f>
+        <v>-28</v>
+      </c>
+      <c r="K15">
+        <f>n*-gap+d</f>
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <f>(p*-gap)+f</f>
+        <v>25</v>
+      </c>
+      <c r="M15">
+        <f>(s*-gap)+h</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-20</v>
+      </c>
+      <c r="E16">
+        <v>-11</v>
+      </c>
+      <c r="F16">
+        <f>m*gap+k</f>
+        <v>-23</v>
+      </c>
+      <c r="G16">
+        <f>o*gap+e</f>
+        <v>-37</v>
+      </c>
+      <c r="H16">
+        <f>q*gap+g</f>
+        <v>-26</v>
+      </c>
+      <c r="K16">
+        <f>n*-gap+d</f>
+        <v>7.5</v>
+      </c>
+      <c r="L16">
+        <f>(p*-gap)+f</f>
+        <v>22.5</v>
+      </c>
+      <c r="M16">
+        <f>(s*-gap)+h</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="E17">
+        <v>-10</v>
+      </c>
+      <c r="F17">
+        <f>m*gap+k</f>
+        <v>-21</v>
+      </c>
+      <c r="G17">
+        <f>o*gap+e</f>
+        <v>-35</v>
+      </c>
+      <c r="H17">
+        <f>q*gap+g</f>
+        <v>-24</v>
+      </c>
+      <c r="K17">
+        <f>n*-gap+d</f>
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f>(p*-gap)+f</f>
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <f>(s*-gap)+h</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>-9</v>
+      </c>
+      <c r="F18">
+        <f>m*gap+k</f>
+        <v>-19</v>
+      </c>
+      <c r="G18">
+        <f>o*gap+e</f>
+        <v>-33</v>
+      </c>
+      <c r="H18">
+        <f>q*gap+g</f>
+        <v>-22</v>
+      </c>
+      <c r="K18">
+        <f>n*-gap+d</f>
+        <v>2.5</v>
+      </c>
+      <c r="L18">
+        <f>(p*-gap)+f</f>
+        <v>17.5</v>
+      </c>
+      <c r="M18">
+        <f>(s*-gap)+h</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-15</v>
+      </c>
+      <c r="E19">
+        <v>-8</v>
+      </c>
+      <c r="F19">
+        <f>m*gap+k</f>
+        <v>-17</v>
+      </c>
+      <c r="G19">
+        <f>o*gap+e</f>
+        <v>-31</v>
+      </c>
+      <c r="H19">
+        <f>q*gap+g</f>
+        <v>-20</v>
+      </c>
+      <c r="K19">
+        <f>n*-gap+d</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>(p*-gap)+f</f>
+        <v>15</v>
+      </c>
+      <c r="M19">
+        <f>(s*-gap)+h</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="E20">
+        <v>-7</v>
+      </c>
+      <c r="F20">
+        <f>m*gap+k</f>
+        <v>-15</v>
+      </c>
+      <c r="G20">
+        <f>o*gap+e</f>
+        <v>-29</v>
+      </c>
+      <c r="H20">
+        <f>q*gap+g</f>
+        <v>-18</v>
+      </c>
+      <c r="K20">
+        <f>n*-gap+d</f>
+        <v>-2.5</v>
+      </c>
+      <c r="L20">
+        <f>(p*-gap)+f</f>
+        <v>12.5</v>
+      </c>
+      <c r="M20">
+        <f>(s*-gap)+h</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="E21">
+        <v>-6</v>
+      </c>
+      <c r="F21">
+        <f>m*gap+k</f>
+        <v>-13</v>
+      </c>
+      <c r="G21">
+        <f>o*gap+e</f>
+        <v>-27</v>
+      </c>
+      <c r="H21">
+        <f>q*gap+g</f>
+        <v>-16</v>
+      </c>
+      <c r="K21">
+        <f>n*-gap+d</f>
+        <v>-5</v>
+      </c>
+      <c r="L21">
+        <f>(p*-gap)+f</f>
+        <v>10</v>
+      </c>
+      <c r="M21">
+        <f>(s*-gap)+h</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>-5</v>
+      </c>
+      <c r="E22">
+        <v>-5</v>
+      </c>
+      <c r="F22">
+        <f>m*gap+k</f>
+        <v>-11</v>
+      </c>
+      <c r="G22">
+        <f>o*gap+e</f>
+        <v>-25</v>
+      </c>
+      <c r="H22">
+        <f>q*gap+g</f>
+        <v>-14</v>
+      </c>
+      <c r="K22">
+        <f>n*-gap+d</f>
+        <v>-7.5</v>
+      </c>
+      <c r="L22">
+        <f>(p*-gap)+f</f>
+        <v>7.5</v>
+      </c>
+      <c r="M22">
+        <f>(s*-gap)+h</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="E23">
+        <v>-4</v>
+      </c>
+      <c r="F23">
+        <f>m*gap+k</f>
+        <v>-9</v>
+      </c>
+      <c r="G23">
+        <f>o*gap+e</f>
+        <v>-23</v>
+      </c>
+      <c r="H23">
+        <f>q*gap+g</f>
+        <v>-12</v>
+      </c>
+      <c r="K23">
+        <f>n*-gap+d</f>
+        <v>-10</v>
+      </c>
+      <c r="L23">
+        <f>(p*-gap)+f</f>
+        <v>5</v>
+      </c>
+      <c r="M23">
+        <f>(s*-gap)+h</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+      <c r="C24" s="8">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>-3</v>
+      </c>
+      <c r="F24">
+        <f>m*gap+k</f>
+        <v>-7</v>
+      </c>
+      <c r="G24">
+        <f>o*gap+e</f>
+        <v>-21</v>
+      </c>
+      <c r="H24">
+        <f>q*gap+g</f>
+        <v>-10</v>
+      </c>
+      <c r="K24">
+        <f>n*-gap+d</f>
+        <v>-12.5</v>
+      </c>
+      <c r="L24">
+        <f>(p*-gap)+f</f>
+        <v>2.5</v>
+      </c>
+      <c r="M24">
+        <f>(s*-gap)+h</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="C25" s="8">
+        <v>-4</v>
+      </c>
+      <c r="E25">
+        <v>-2</v>
+      </c>
+      <c r="F25">
+        <f>m*gap+k</f>
+        <v>-5</v>
+      </c>
+      <c r="G25">
+        <f>o*gap+e</f>
+        <v>-19</v>
+      </c>
+      <c r="H25">
+        <f>q*gap+g</f>
+        <v>-8</v>
+      </c>
+      <c r="K25">
+        <f>n*-gap+d</f>
+        <v>-15</v>
+      </c>
+      <c r="L25">
+        <f>(p*-gap)+f</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>(s*-gap)+h</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="E26">
+        <v>-1</v>
+      </c>
+      <c r="F26">
+        <f>m*gap+k</f>
+        <v>-3</v>
+      </c>
+      <c r="G26">
+        <f>o*gap+e</f>
+        <v>-17</v>
+      </c>
+      <c r="H26">
+        <f>q*gap+g</f>
+        <v>-6</v>
+      </c>
+      <c r="K26">
+        <f>n*-gap+d</f>
+        <v>-17.5</v>
+      </c>
+      <c r="L26">
+        <f>(p*-gap)+f</f>
+        <v>-2.5</v>
+      </c>
+      <c r="M26">
+        <f>(s*-gap)+h</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>m*gap+k</f>
+        <v>-1</v>
+      </c>
+      <c r="G27">
+        <f>o*gap+e</f>
+        <v>-15</v>
+      </c>
+      <c r="H27">
+        <f>q*gap+g</f>
+        <v>-4</v>
+      </c>
+      <c r="K27">
+        <f>n*-gap+d</f>
+        <v>-20</v>
+      </c>
+      <c r="L27">
+        <f>(p*-gap)+f</f>
+        <v>-5</v>
+      </c>
+      <c r="M27">
+        <f>(s*-gap)+h</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
+      <c r="C28" s="8">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f>m*gap+k</f>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f>o*gap+e</f>
+        <v>-13</v>
+      </c>
+      <c r="H28">
+        <f>q*gap+g</f>
+        <v>-2</v>
+      </c>
+      <c r="K28">
+        <f>n*-gap+d</f>
+        <v>-22.5</v>
+      </c>
+      <c r="L28">
+        <f>(p*-gap)+f</f>
+        <v>-7.5</v>
+      </c>
+      <c r="M28">
+        <f>(s*-gap)+h</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <f>m*gap+k</f>
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <f>o*gap+e</f>
+        <v>-11</v>
+      </c>
+      <c r="H29">
+        <f>q*gap+g</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>n*-gap+d</f>
+        <v>-25</v>
+      </c>
+      <c r="L29">
+        <f>(p*-gap)+f</f>
+        <v>-10</v>
+      </c>
+      <c r="M29">
+        <f>(s*-gap)+h</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f>m*gap+k</f>
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <f>o*gap+e</f>
+        <v>-9</v>
+      </c>
+      <c r="H30">
+        <f>q*gap+g</f>
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <f>n*-gap+d</f>
+        <v>-27.5</v>
+      </c>
+      <c r="L30">
+        <f>(p*-gap)+f</f>
+        <v>-12.5</v>
+      </c>
+      <c r="M30">
+        <f>(s*-gap)+h</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <f>m*gap+k</f>
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <f>o*gap+e</f>
+        <v>-7</v>
+      </c>
+      <c r="H31">
+        <f>q*gap+g</f>
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <f>n*-gap+d</f>
+        <v>-30</v>
+      </c>
+      <c r="L31">
+        <f>(p*-gap)+f</f>
+        <v>-15</v>
+      </c>
+      <c r="M31">
+        <f>(s*-gap)+h</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <f>m*gap+k</f>
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <f>o*gap+e</f>
+        <v>-5</v>
+      </c>
+      <c r="H32">
+        <f>q*gap+g</f>
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <f>n*-gap+d</f>
+        <v>-32.5</v>
+      </c>
+      <c r="L32">
+        <f>(p*-gap)+f</f>
+        <v>-17.5</v>
+      </c>
+      <c r="M32">
+        <f>(s*-gap)+h</f>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <f>m*gap+k</f>
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <f>o*gap+e</f>
+        <v>-3</v>
+      </c>
+      <c r="H33">
+        <f>q*gap+g</f>
+        <v>8</v>
+      </c>
+      <c r="K33">
+        <f>n*-gap+d</f>
+        <v>-35</v>
+      </c>
+      <c r="L33">
+        <f>(p*-gap)+f</f>
+        <v>-20</v>
+      </c>
+      <c r="M33">
+        <f>(s*-gap)+h</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="11"/>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f>m*gap+k</f>
+        <v>13</v>
+      </c>
+      <c r="G34">
+        <f>o*gap+e</f>
+        <v>-1</v>
+      </c>
+      <c r="H34">
+        <f>q*gap+g</f>
+        <v>10</v>
+      </c>
+      <c r="K34">
+        <f>n*-gap+d</f>
+        <v>-37.5</v>
+      </c>
+      <c r="L34">
+        <f>(p*-gap)+f</f>
+        <v>-22.5</v>
+      </c>
+      <c r="M34">
+        <f>(s*-gap)+h</f>
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="B35" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <f>m*gap+k</f>
+        <v>15</v>
+      </c>
+      <c r="G35">
+        <f>o*gap+e</f>
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H35">
+        <f>q*gap+g</f>
+        <v>12</v>
+      </c>
+      <c r="K35">
+        <f>n*-gap+d</f>
+        <v>-40</v>
+      </c>
+      <c r="L35">
+        <f>(p*-gap)+f</f>
+        <v>-25</v>
+      </c>
+      <c r="M35">
+        <f>(s*-gap)+h</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="29"/>
+      <c r="B36" s="28">
+        <f>D1</f>
+        <v>-4.2222222222222223</v>
+      </c>
+      <c r="C36" s="2">
+        <v>-25</v>
+      </c>
+      <c r="E36">
         <v>9</v>
       </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="F36">
+        <f>m*gap+k</f>
+        <v>17</v>
+      </c>
+      <c r="G36">
+        <f>o*gap+e</f>
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <f>q*gap+g</f>
+        <v>14</v>
+      </c>
+      <c r="K36">
+        <f>n*-gap+d</f>
+        <v>-42.5</v>
+      </c>
+      <c r="L36">
+        <f>(p*-gap)+f</f>
+        <v>-27.5</v>
+      </c>
+      <c r="M36">
+        <f>(s*-gap)+h</f>
+        <v>-12.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="29"/>
+      <c r="B37" s="28">
+        <f>D1</f>
+        <v>-4.2222222222222223</v>
+      </c>
+      <c r="C37" s="2">
+        <f>D2</f>
+        <v>-9.4444444444444446</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <f>m*gap+k</f>
+        <v>19</v>
+      </c>
+      <c r="G37">
+        <f>o*gap+e</f>
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <f>q*gap+g</f>
+        <v>16</v>
+      </c>
+      <c r="K37">
+        <f>n*-gap+d</f>
+        <v>-45</v>
+      </c>
+      <c r="L37">
+        <f>(p*-gap)+f</f>
+        <v>-30</v>
+      </c>
+      <c r="M37">
+        <f>(s*-gap)+h</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="29"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="22"/>
+      <c r="E38">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E10">
-        <v>-15</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ref="F10:F17" si="0">$C$12*E10+$C$13</f>
+      <c r="F38">
+        <f>m*gap+k</f>
+        <v>21</v>
+      </c>
+      <c r="G38">
+        <f>o*gap+e</f>
+        <v>7</v>
+      </c>
+      <c r="H38">
+        <f>q*gap+g</f>
+        <v>18</v>
+      </c>
+      <c r="K38">
+        <f>n*-gap+d</f>
+        <v>-47.5</v>
+      </c>
+      <c r="L38">
+        <f>(p*-gap)+f</f>
+        <v>-32.5</v>
+      </c>
+      <c r="M38">
+        <f>(s*-gap)+h</f>
+        <v>-17.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="29"/>
+      <c r="B39" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f>m*gap+k</f>
+        <v>23</v>
+      </c>
+      <c r="G39">
+        <f>o*gap+e</f>
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <f>q*gap+g</f>
+        <v>20</v>
+      </c>
+      <c r="K39">
+        <f>n*-gap+d</f>
+        <v>-50</v>
+      </c>
+      <c r="L39">
+        <f>(p*-gap)+f</f>
+        <v>-35</v>
+      </c>
+      <c r="M39">
+        <f>(s*-gap)+h</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="29"/>
+      <c r="B40" s="28">
+        <f>C36</f>
+        <v>-25</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C37</f>
+        <v>-9.4444444444444446</v>
+      </c>
+      <c r="E40">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <f>m*gap+k</f>
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <f>o*gap+e</f>
+        <v>11</v>
+      </c>
+      <c r="H40">
+        <f>q*gap+g</f>
+        <v>22</v>
+      </c>
+      <c r="K40">
+        <f>n*-gap+d</f>
+        <v>-52.5</v>
+      </c>
+      <c r="L40">
+        <f>(p*-gap)+f</f>
+        <v>-37.5</v>
+      </c>
+      <c r="M40">
+        <f>(s*-gap)+h</f>
+        <v>-22.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="29"/>
+      <c r="B41" s="28">
+        <f>D1</f>
+        <v>-4.2222222222222223</v>
+      </c>
+      <c r="C41" s="2">
+        <f>C40</f>
+        <v>-9.4444444444444446</v>
+      </c>
+      <c r="E41">
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <f>m*gap+k</f>
+        <v>27</v>
+      </c>
+      <c r="G41">
+        <f>o*gap+e</f>
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <f>q*gap+g</f>
+        <v>24</v>
+      </c>
+      <c r="K41">
+        <f>n*-gap+d</f>
+        <v>-55</v>
+      </c>
+      <c r="L41">
+        <f>(p*-gap)+f</f>
         <v>-40</v>
       </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G17" si="1">$C$18*E10+$C$19</f>
-        <v>-45</v>
-      </c>
-      <c r="K10">
-        <f t="shared" ref="K10:K17" si="2">$C$15*-E10+$C$16</f>
-        <v>17.5</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ref="L10:L17" si="3">($C$21*-E10)+$C$22</f>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E11">
-        <v>-14</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>-38</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
-        <v>-43</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="2"/>
+      <c r="M41">
+        <f>(s*-gap)+h</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E42">
         <v>15</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>-13</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>-36</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="1"/>
-        <v>-41</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>-10</v>
-      </c>
-      <c r="E13">
-        <v>-12</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>-34</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>-39</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="2"/>
+      <c r="F42">
+        <f>m*gap+k</f>
+        <v>29</v>
+      </c>
+      <c r="G42">
+        <f>o*gap+e</f>
+        <v>15</v>
+      </c>
+      <c r="H42">
+        <f>q*gap+g</f>
+        <v>26</v>
+      </c>
+      <c r="K42">
+        <f>n*-gap+d</f>
+        <v>-57.5</v>
+      </c>
+      <c r="L42">
+        <f>(p*-gap)+f</f>
+        <v>-42.5</v>
+      </c>
+      <c r="M42">
+        <f>(s*-gap)+h</f>
+        <v>-27.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="31">
+        <f>D4</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="C44" s="5">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="31">
+        <f>D4</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="C45" s="5">
+        <f>D5</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="23"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E14">
-        <v>-11</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>-32</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
-        <v>-37</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="2"/>
-        <v>7.5</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>2.5</v>
-      </c>
-      <c r="E15">
-        <v>-10</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>-30</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>-35</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="30">
+        <f>C44</f>
+        <v>-25</v>
+      </c>
+      <c r="C48" s="5">
+        <f>D5</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="31">
+        <f>D4</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="C49" s="5">
+        <f>D5</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="34"/>
+      <c r="B52" s="33">
+        <f>D7</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C52" s="8">
+        <f>C36</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="34"/>
+      <c r="B53" s="33">
+        <f>D7</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C53" s="8">
+        <f>D8</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="34"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="24"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="34"/>
+      <c r="B55" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>-20</v>
-      </c>
-      <c r="E16">
-        <v>-9</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>-28</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="1"/>
-        <v>-33</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E17">
-        <v>-8</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>-26</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>-31</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="2"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="34"/>
+      <c r="B56" s="33">
+        <f>C52</f>
+        <v>-25</v>
+      </c>
+      <c r="C56" s="8">
+        <f>D8</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="34"/>
+      <c r="B57" s="33">
+        <f>D7</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C57" s="8">
+        <f>D8</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>-7</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F32" si="4">$C$12*E18+$C$13</f>
-        <v>-24</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ref="G18:G32" si="5">$C$18*E18+$C$19</f>
-        <v>-29</v>
-      </c>
-      <c r="K18">
-        <f t="shared" ref="K18:K32" si="6">$C$15*-E18+$C$16</f>
-        <v>-2.5</v>
-      </c>
-      <c r="L18">
-        <f t="shared" ref="L18:L32" si="7">($C$21*-E18)+$C$22</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>-15</v>
-      </c>
-      <c r="E19">
-        <v>-6</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>-22</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>-27</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="6"/>
-        <v>-5</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="7"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="14"/>
+      <c r="B61" s="2">
+        <f>D1</f>
+        <v>-4.2222222222222223</v>
+      </c>
+      <c r="C61" s="2">
+        <f>D2</f>
+        <v>-9.4444444444444446</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="15"/>
+      <c r="B62" s="2">
+        <f>D1</f>
+        <v>-4.2222222222222223</v>
+      </c>
+      <c r="C62" s="2">
+        <f>D2</f>
+        <v>-9.4444444444444446</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E20">
-        <v>-5</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>-20</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="5"/>
-        <v>-25</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="6"/>
-        <v>-7.5</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="7"/>
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>2.5</v>
-      </c>
-      <c r="E21">
-        <v>-4</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>-18</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="5"/>
-        <v>-23</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="6"/>
-        <v>-10</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="7"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22">
-        <v>-15</v>
-      </c>
-      <c r="E22">
-        <v>-3</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>-16</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="5"/>
-        <v>-21</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="6"/>
-        <v>-12.5</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="7"/>
-        <v>-7.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E23">
-        <v>-2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
-        <v>-14</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="5"/>
-        <v>-19</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="6"/>
-        <v>-15</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="7"/>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E24">
-        <v>-1</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>-12</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>-17</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="6"/>
-        <v>-17.5</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="7"/>
-        <v>-12.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="17"/>
+      <c r="B65" s="12">
+        <f>D4</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="C65" s="5">
+        <f>D5</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="18"/>
+      <c r="B66" s="12">
+        <f>D4</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="C66" s="5">
+        <f>D5</f>
+        <v>-10.555555555555555</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>-10</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="5"/>
-        <v>-15</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="6"/>
-        <v>-20</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="7"/>
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
-        <v>-8</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="5"/>
-        <v>-13</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="6"/>
-        <v>-22.5</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="7"/>
-        <v>-17.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
-        <v>-6</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="5"/>
-        <v>-11</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="6"/>
-        <v>-25</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="7"/>
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f>($C$16-$C$13)/($C$12-$C$15)</f>
-        <v>20</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
-        <v>-4</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="5"/>
-        <v>-9</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="6"/>
-        <v>-27.5</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="7"/>
-        <v>-22.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <f>($C$12*$C$28)+$C$13</f>
-        <v>30</v>
-      </c>
-      <c r="E29">
-        <v>4</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
-        <v>-2</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="5"/>
-        <v>-7</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="6"/>
-        <v>-30</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="7"/>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E30">
-        <v>5</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="5"/>
-        <v>-5</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="6"/>
-        <v>-32.5</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="7"/>
-        <v>-27.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>6</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="5"/>
-        <v>-3</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="6"/>
-        <v>-35</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="7"/>
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <f>C28</f>
-        <v>20</v>
-      </c>
-      <c r="C32">
-        <f>C29</f>
-        <v>30</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="6"/>
-        <v>-37.5</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="7"/>
-        <v>-32.5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <f>C32</f>
-        <v>30</v>
-      </c>
-      <c r="E33">
-        <v>8</v>
-      </c>
-      <c r="F33">
-        <f t="shared" ref="F33:F40" si="8">$C$12*E33+$C$13</f>
-        <v>6</v>
-      </c>
-      <c r="G33">
-        <f t="shared" ref="G33:G40" si="9">$C$18*E33+$C$19</f>
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <f t="shared" ref="K33:K40" si="10">$C$15*-E33+$C$16</f>
-        <v>-40</v>
-      </c>
-      <c r="L33">
-        <f t="shared" ref="L33:L40" si="11">($C$21*-E33)+$C$22</f>
-        <v>-35</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E34">
-        <v>9</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="10"/>
-        <v>-42.5</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="11"/>
-        <v>-37.5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E35">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="10"/>
-        <v>-45</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="11"/>
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E36">
-        <v>11</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="10"/>
-        <v>-47.5</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="11"/>
-        <v>-42.5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E37">
-        <v>12</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="10"/>
-        <v>-50</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="11"/>
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E38">
-        <v>13</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="10"/>
-        <v>-52.5</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="11"/>
-        <v>-47.5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E39">
-        <v>14</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="9"/>
-        <v>13</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="10"/>
-        <v>-55</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="11"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E40">
-        <v>15</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="9"/>
-        <v>15</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="10"/>
-        <v>-57.5</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="11"/>
-        <v>-52.5</v>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="20"/>
+      <c r="B69" s="8">
+        <f>D7</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C69" s="8">
+        <f>D8</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="21"/>
+      <c r="B70" s="8">
+        <f>D7</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C70" s="8">
+        <f>D8</f>
+        <v>2.2222222222222223</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A26:D26"/>
+  <mergeCells count="17">
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Tamabahan sofie-npi dan sofie-isma
</commit_message>
<xml_diff>
--- a/doc/Coba Stylized Fact.xlsx
+++ b/doc/Coba Stylized Fact.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerja Bismillah\DKEM\Riset dan Kajian\KajianFPP\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4694D3B1-60E6-461B-87C5-397AA3E68DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215D5C6D-F9C5-45DD-83A0-6DF1B860222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB5E76F9-A705-4992-8E41-F9C5477B9BFA}"/>
   </bookViews>
@@ -277,32 +277,27 @@
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,24 +325,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3622,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A975199-FB5E-4713-850D-869388F6B6C9}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3632,76 +3632,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <f>(-k + d)/(m+n)</f>
         <v>-4.2222222222222223</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="15"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <f>m*((-k + d)/(m+n))+k</f>
         <v>-9.4444444444444446</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="5">
         <f xml:space="preserve"> (-e+f)/(o+p)</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <f xml:space="preserve"> o*((-e+f)/(o+p)) + e</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="3">
         <f>(-g + h)/(q+s)</f>
         <v>3.1111111111111112</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="21"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="3">
         <f>q*((-g + h)/(q+s))+g</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="32"/>
       <c r="E11" t="s">
         <v>13</v>
       </c>
@@ -3725,581 +3725,581 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="E12">
         <v>-15</v>
       </c>
       <c r="F12">
-        <f>m*gap+k</f>
+        <f t="shared" ref="F12:F42" si="0">m*gap+k</f>
         <v>-31</v>
       </c>
       <c r="G12">
-        <f>o*gap+e</f>
+        <f t="shared" ref="G12:G42" si="1">o*gap+e</f>
         <v>-45</v>
       </c>
       <c r="H12">
-        <f>q*gap+g</f>
+        <f t="shared" ref="H12:H42" si="2">q*gap+g</f>
         <v>-34</v>
       </c>
       <c r="K12">
-        <f>n*-gap+d</f>
+        <f t="shared" ref="K12:K42" si="3">n*-gap+d</f>
         <v>17.5</v>
       </c>
       <c r="L12">
-        <f>(p*-gap)+f</f>
+        <f t="shared" ref="L12:L42" si="4">(p*-gap)+f</f>
         <v>32.5</v>
       </c>
       <c r="M12">
-        <f>(s*-gap)+h</f>
+        <f t="shared" ref="M12:M42" si="5">(s*-gap)+h</f>
         <v>47.5</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>-1</v>
       </c>
       <c r="E13">
         <v>-14</v>
       </c>
       <c r="F13">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-29</v>
       </c>
       <c r="G13">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-43</v>
       </c>
       <c r="H13">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-32</v>
       </c>
       <c r="K13">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="L13">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="M13">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
       <c r="E14">
         <v>-13</v>
       </c>
       <c r="F14">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-27</v>
       </c>
       <c r="G14">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-41</v>
       </c>
       <c r="H14">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-30</v>
       </c>
       <c r="K14">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="L14">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>27.5</v>
       </c>
       <c r="M14">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>42.5</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>2.5</v>
       </c>
       <c r="E15">
         <v>-12</v>
       </c>
       <c r="F15">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-25</v>
       </c>
       <c r="G15">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-39</v>
       </c>
       <c r="H15">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-28</v>
       </c>
       <c r="K15">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L15">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="M15">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>-20</v>
       </c>
       <c r="E16">
         <v>-11</v>
       </c>
       <c r="F16">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-23</v>
       </c>
       <c r="G16">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-37</v>
       </c>
       <c r="H16">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-26</v>
       </c>
       <c r="K16">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
       <c r="L16">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>22.5</v>
       </c>
       <c r="M16">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="34"/>
       <c r="E17">
         <v>-10</v>
       </c>
       <c r="F17">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-21</v>
       </c>
       <c r="G17">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-35</v>
       </c>
       <c r="H17">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="K17">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L17">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="M17">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>2</v>
       </c>
       <c r="E18">
         <v>-9</v>
       </c>
       <c r="F18">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-19</v>
       </c>
       <c r="G18">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-33</v>
       </c>
       <c r="H18">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-22</v>
       </c>
       <c r="K18">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
       <c r="L18">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>17.5</v>
       </c>
       <c r="M18">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>32.5</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="2">
         <v>-15</v>
       </c>
       <c r="E19">
         <v>-8</v>
       </c>
       <c r="F19">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-17</v>
       </c>
       <c r="G19">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-31</v>
       </c>
       <c r="H19">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-20</v>
       </c>
       <c r="K19">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L19">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="M19">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
       <c r="E20">
         <v>-7</v>
       </c>
       <c r="F20">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-15</v>
       </c>
       <c r="G20">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-29</v>
       </c>
       <c r="H20">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-18</v>
       </c>
       <c r="K20">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-2.5</v>
       </c>
       <c r="L20">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
       <c r="M20">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>27.5</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <v>2.5</v>
       </c>
       <c r="E21">
         <v>-6</v>
       </c>
       <c r="F21">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-13</v>
       </c>
       <c r="G21">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-27</v>
       </c>
       <c r="H21">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="K21">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L21">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="M21">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="2">
         <v>-5</v>
       </c>
       <c r="E22">
         <v>-5</v>
       </c>
       <c r="F22">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="G22">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
       <c r="H22">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-14</v>
       </c>
       <c r="K22">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-7.5</v>
       </c>
       <c r="L22">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
       <c r="M22">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>22.5</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="17"/>
       <c r="E23">
         <v>-4</v>
       </c>
       <c r="F23">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
       <c r="G23">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-23</v>
       </c>
       <c r="H23">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="K23">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="L23">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="M23">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="E24">
         <v>-3</v>
       </c>
       <c r="F24">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="G24">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-21</v>
       </c>
       <c r="H24">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="K24">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-12.5</v>
       </c>
       <c r="L24">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="M24">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>17.5</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="3">
         <v>-4</v>
       </c>
       <c r="E25">
         <v>-2</v>
       </c>
       <c r="F25">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
       <c r="G25">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-19</v>
       </c>
       <c r="H25">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="K25">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-15</v>
       </c>
       <c r="L25">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M25">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
       <c r="E26">
         <v>-1</v>
       </c>
       <c r="F26">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="G26">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-17</v>
       </c>
       <c r="H26">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="K26">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-17.5</v>
       </c>
       <c r="L26">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-2.5</v>
       </c>
       <c r="M26">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="3">
         <v>2.5</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="G27">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-15</v>
       </c>
       <c r="H27">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="K27">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-20</v>
       </c>
       <c r="L27">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="M27">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="3">
         <v>10</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G28">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-13</v>
       </c>
       <c r="H28">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="K28">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-22.5</v>
       </c>
       <c r="L28">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-7.5</v>
       </c>
       <c r="M28">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>7.5</v>
       </c>
     </row>
@@ -4308,27 +4308,27 @@
         <v>2</v>
       </c>
       <c r="F29">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G29">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="H29">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K29">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-25</v>
       </c>
       <c r="L29">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-10</v>
       </c>
       <c r="M29">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -4337,27 +4337,27 @@
         <v>3</v>
       </c>
       <c r="F30">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G30">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="H30">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K30">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-27.5</v>
       </c>
       <c r="L30">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-12.5</v>
       </c>
       <c r="M30">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
     </row>
@@ -4366,27 +4366,27 @@
         <v>4</v>
       </c>
       <c r="F31">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G31">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-7</v>
       </c>
       <c r="H31">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K31">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-30</v>
       </c>
       <c r="L31">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-15</v>
       </c>
       <c r="M31">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4395,27 +4395,27 @@
         <v>5</v>
       </c>
       <c r="F32">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G32">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="H32">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K32">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-32.5</v>
       </c>
       <c r="L32">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-17.5</v>
       </c>
       <c r="M32">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-2.5</v>
       </c>
     </row>
@@ -4424,62 +4424,62 @@
         <v>6</v>
       </c>
       <c r="F33">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G33">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="H33">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K33">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-35</v>
       </c>
       <c r="L33">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-20</v>
       </c>
       <c r="M33">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-5</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="11"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="4"/>
       <c r="E34">
         <v>7</v>
       </c>
       <c r="F34">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G34">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="H34">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="K34">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-37.5</v>
       </c>
       <c r="L34">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-22.5</v>
       </c>
       <c r="M34">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-7.5</v>
       </c>
     </row>
@@ -4487,84 +4487,84 @@
       <c r="A35" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E35">
         <v>8</v>
       </c>
       <c r="F35">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G35">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H35">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="K35">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="L35">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-25</v>
       </c>
       <c r="M35">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-10</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
-      <c r="B36" s="28">
+      <c r="B36" s="12">
         <f>D1</f>
         <v>-4.2222222222222223</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>-25</v>
       </c>
       <c r="E36">
         <v>9</v>
       </c>
       <c r="F36">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="G36">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H36">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="K36">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-42.5</v>
       </c>
       <c r="L36">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-27.5</v>
       </c>
       <c r="M36">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-12.5</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
-      <c r="B37" s="28">
+      <c r="B37" s="12">
         <f>D1</f>
         <v>-4.2222222222222223</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <f>D2</f>
         <v>-9.4444444444444446</v>
       </c>
@@ -4572,105 +4572,105 @@
         <v>10</v>
       </c>
       <c r="F37">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="G37">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H37">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K37">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-45</v>
       </c>
       <c r="L37">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-30</v>
       </c>
       <c r="M37">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-15</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="22"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="6"/>
       <c r="E38">
         <v>11</v>
       </c>
       <c r="F38">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="G38">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H38">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="K38">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-47.5</v>
       </c>
       <c r="L38">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-32.5</v>
       </c>
       <c r="M38">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-17.5</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E39">
         <v>12</v>
       </c>
       <c r="F39">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G39">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="H39">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K39">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-50</v>
       </c>
       <c r="L39">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-35</v>
       </c>
       <c r="M39">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-20</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
-      <c r="B40" s="28">
+      <c r="B40" s="12">
         <f>C36</f>
         <v>-25</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <f>C37</f>
         <v>-9.4444444444444446</v>
       </c>
@@ -4678,37 +4678,37 @@
         <v>13</v>
       </c>
       <c r="F40">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G40">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="H40">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="K40">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-52.5</v>
       </c>
       <c r="L40">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-37.5</v>
       </c>
       <c r="M40">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-22.5</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
-      <c r="B41" s="28">
+      <c r="B41" s="12">
         <f>D1</f>
         <v>-4.2222222222222223</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <f>C40</f>
         <v>-9.4444444444444446</v>
       </c>
@@ -4716,27 +4716,27 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="G41">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H41">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="K41">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-55</v>
       </c>
       <c r="L41">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-40</v>
       </c>
       <c r="M41">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-25</v>
       </c>
     </row>
@@ -4745,275 +4745,277 @@
         <v>15</v>
       </c>
       <c r="F42">
-        <f>m*gap+k</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="G42">
-        <f>o*gap+e</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H42">
-        <f>q*gap+g</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="K42">
-        <f>n*-gap+d</f>
+        <f t="shared" si="3"/>
         <v>-57.5</v>
       </c>
       <c r="L42">
-        <f>(p*-gap)+f</f>
+        <f t="shared" si="4"/>
         <v>-42.5</v>
       </c>
       <c r="M42">
-        <f>(s*-gap)+h</f>
+        <f t="shared" si="5"/>
         <v>-27.5</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="31">
+      <c r="A44" s="28"/>
+      <c r="B44" s="14">
         <f>D4</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="2">
         <v>-25</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="31">
+      <c r="A45" s="28"/>
+      <c r="B45" s="14">
         <f>D4</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="2">
         <f>D5</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="32"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="23"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="30" t="s">
+      <c r="A47" s="28"/>
+      <c r="B47" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
-      <c r="B48" s="30">
+      <c r="A48" s="28"/>
+      <c r="B48" s="13">
         <f>C44</f>
         <v>-25</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="2">
         <f>D5</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="31">
+      <c r="A49" s="28"/>
+      <c r="B49" s="14">
         <f>D4</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="2">
         <f>D5</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="34"/>
-      <c r="B52" s="33">
+      <c r="A52" s="27"/>
+      <c r="B52" s="15">
         <f>D7</f>
         <v>3.1111111111111112</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="3">
         <f>C36</f>
         <v>-25</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="34"/>
-      <c r="B53" s="33">
+      <c r="A53" s="27"/>
+      <c r="B53" s="15">
         <f>D7</f>
         <v>3.1111111111111112</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="3">
         <f>D8</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="34"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="24"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="34"/>
-      <c r="B55" s="33" t="s">
+      <c r="A55" s="27"/>
+      <c r="B55" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="34"/>
-      <c r="B56" s="33">
+      <c r="A56" s="27"/>
+      <c r="B56" s="15">
         <f>C52</f>
         <v>-25</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="3">
         <f>D8</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="34"/>
-      <c r="B57" s="33">
+      <c r="A57" s="27"/>
+      <c r="B57" s="15">
         <f>D7</f>
         <v>3.1111111111111112</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="3">
         <f>D8</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="2">
+      <c r="A61" s="19"/>
+      <c r="B61" s="1">
         <f>D1</f>
         <v>-4.2222222222222223</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <f>D2</f>
         <v>-9.4444444444444446</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="15"/>
-      <c r="B62" s="2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="1">
         <f>D1</f>
         <v>-4.2222222222222223</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <f>D2</f>
         <v>-9.4444444444444446</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65" s="12">
+      <c r="A65" s="22"/>
+      <c r="B65" s="5">
         <f>D4</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="2">
         <f>D5</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="12">
+      <c r="A66" s="23"/>
+      <c r="B66" s="5">
         <f>D4</f>
         <v>2.2222222222222223</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="2">
         <f>D5</f>
         <v>-10.555555555555555</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="20"/>
-      <c r="B69" s="8">
+      <c r="A69" s="25"/>
+      <c r="B69" s="3">
         <f>D7</f>
         <v>3.1111111111111112</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C69" s="3">
         <f>D8</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="21"/>
-      <c r="B70" s="8">
+      <c r="A70" s="26"/>
+      <c r="B70" s="3">
         <f>D7</f>
         <v>3.1111111111111112</v>
       </c>
-      <c r="C70" s="8">
+      <c r="C70" s="3">
         <f>D8</f>
         <v>2.2222222222222223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="A64:A66"/>
     <mergeCell ref="A68:A70"/>
@@ -5029,8 +5031,6 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>